<commit_message>
use LSB of the ADV7125 (new design is compatible to initial public N64RGBv2 Version 20171211)
</commit_message>
<xml_diff>
--- a/generalRGBmod/Main-PCB/v2/BOM_n64rgbv2.xlsx
+++ b/generalRGBmod/Main-PCB/v2/BOM_n64rgbv2.xlsx
@@ -15,7 +15,7 @@
     <sheet name="MaxV Setup" sheetId="1" r:id="rId1"/>
     <sheet name="MaxII Setup" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="98">
   <si>
     <t>Designator</t>
   </si>
@@ -102,15 +102,6 @@
     <t>1.8V LDO regulator</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>(Jumper)</t>
-  </si>
-  <si>
-    <t>Leave J1 open</t>
-  </si>
-  <si>
     <t>ICs and Regulators</t>
   </si>
   <si>
@@ -327,10 +318,10 @@
     <t xml:space="preserve">EPM240T100C5N </t>
   </si>
   <si>
-    <t>Close J1</t>
-  </si>
-  <si>
     <t>C2,C3,C31</t>
+  </si>
+  <si>
+    <t>FB1,FB2,FB3</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1160,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1208,7 +1199,7 @@
     <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1241,7 +1232,7 @@
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1251,19 +1242,19 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1273,17 +1264,17 @@
         <v>20</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="1"/>
@@ -1291,7 +1282,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -1311,24 +1302,20 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="G9" s="7"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1339,88 +1326,97 @@
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s">
+        <v>52</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>35</v>
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" t="s">
+        <v>52</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1430,16 +1426,16 @@
         <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C17">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
@@ -1449,32 +1445,32 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1483,51 +1479,51 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
+        <v>92</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
         <v>11</v>
@@ -1537,19 +1533,19 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
         <v>36</v>
       </c>
-      <c r="B22" t="s">
-        <v>95</v>
-      </c>
       <c r="C22" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s">
         <v>11</v>
@@ -1559,13 +1555,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="C23" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -1581,66 +1577,66 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="7">
+        <v>77</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
-      <c r="E24" t="s">
-        <v>45</v>
+      <c r="E24" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="F24" t="s">
         <v>11</v>
       </c>
+      <c r="G24" t="s">
+        <v>80</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="7">
+        <v>2</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>82</v>
+      <c r="E25" t="s">
+        <v>40</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
       </c>
-      <c r="G25" t="s">
-        <v>83</v>
-      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C26" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F26" t="s">
         <v>11</v>
@@ -1650,19 +1646,19 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="7">
+        <v>75</v>
+      </c>
+      <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
       </c>
-      <c r="E27" t="s">
-        <v>44</v>
+      <c r="E27" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="F27" t="s">
         <v>11</v>
@@ -1672,41 +1668,41 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="D29" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="F29" t="s">
         <v>8</v>
@@ -1715,123 +1711,101 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F30" t="s">
-        <v>8</v>
-      </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>82</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>86</v>
-      </c>
-      <c r="B32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="G32" t="s">
-        <v>85</v>
-      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
+      <c r="E37" s="3"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
-      <c r="E38" s="3"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
+      <c r="E39" s="3"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="3"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E41" s="3"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E42" s="3"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="3"/>
       <c r="G43" s="2"/>
       <c r="H43" s="4"/>
-      <c r="I43" s="5"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E44" s="3"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A33:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1879,7 +1853,7 @@
     <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1887,7 +1861,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1903,7 +1877,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
@@ -1912,7 +1886,7 @@
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1922,19 +1896,19 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1944,36 +1918,30 @@
         <v>20</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="6" t="s">
-        <v>99</v>
-      </c>
+      <c r="G8" s="6"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
@@ -1990,7 +1958,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -2003,10 +1971,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2015,26 +1983,26 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
@@ -2048,17 +2016,17 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -2067,20 +2035,20 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -2089,7 +2057,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
@@ -2099,10 +2067,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -2111,7 +2079,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
@@ -2121,10 +2089,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2133,20 +2101,20 @@
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2155,7 +2123,7 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
@@ -2165,10 +2133,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C20" s="7">
         <v>1</v>
@@ -2177,7 +2145,7 @@
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
         <v>11</v>
@@ -2187,10 +2155,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C21" s="7">
         <v>2</v>
@@ -2199,7 +2167,7 @@
         <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s">
         <v>11</v>
@@ -2209,10 +2177,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C22" s="7">
         <v>1</v>
@@ -2221,7 +2189,7 @@
         <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F22" t="s">
         <v>11</v>
@@ -2231,10 +2199,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2243,23 +2211,23 @@
         <v>12</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F23" t="s">
         <v>11</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C24" s="7">
         <v>2</v>
@@ -2268,7 +2236,7 @@
         <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s">
         <v>11</v>
@@ -2278,10 +2246,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
@@ -2290,7 +2258,7 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F25" t="s">
         <v>11</v>
@@ -2300,10 +2268,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2312,7 +2280,7 @@
         <v>12</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F26" t="s">
         <v>11</v>
@@ -2322,19 +2290,19 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
@@ -2344,19 +2312,19 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
@@ -2370,16 +2338,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>

</xml_diff>